<commit_message>
Commit après modification algorithme et interface
</commit_message>
<xml_diff>
--- a/Composants.xlsx
+++ b/Composants.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remy\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Composants" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -83,8 +81,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +94,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,9 +129,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -125,9 +141,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="NiveauLigne_4" xfId="1" builtinId="1" iLevel="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="RowLevel_4" xfId="1" builtinId="1" iLevel="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -185,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -237,7 +255,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -431,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -439,19 +457,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D16"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -470,10 +488,13 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,8 +504,11 @@
       <c r="C3">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -494,8 +518,11 @@
       <c r="C4">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -505,8 +532,11 @@
       <c r="C5">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -514,10 +544,13 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -527,8 +560,11 @@
       <c r="C7">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -538,8 +574,11 @@
       <c r="C8">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -547,10 +586,13 @@
         <v>10</v>
       </c>
       <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="E9">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -560,8 +602,11 @@
       <c r="C10">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -569,10 +614,13 @@
         <v>12</v>
       </c>
       <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="E11">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -582,8 +630,11 @@
       <c r="C12">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -593,8 +644,11 @@
       <c r="C13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -604,8 +658,11 @@
       <c r="C14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -615,8 +672,11 @@
       <c r="C15">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -624,10 +684,19 @@
         <v>17</v>
       </c>
       <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="E16">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>